<commit_message>
modify allow-gold as 10000
</commit_message>
<xml_diff>
--- a/app/scripts/data/jobs.xlsx
+++ b/app/scripts/data/jobs.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="18945" windowHeight="7425" activeTab="2"/>
+    <workbookView windowWidth="20700" windowHeight="9870"/>
   </bookViews>
   <sheets>
     <sheet name="jobs" sheetId="1" r:id="rId1"/>
@@ -1114,8 +1114,8 @@
   <sheetPr/>
   <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2:D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelCol="4"/>
@@ -1153,7 +1153,7 @@
         <v>6</v>
       </c>
       <c r="D2">
-        <v>100</v>
+        <v>10000</v>
       </c>
       <c r="E2">
         <v>21</v>
@@ -1170,7 +1170,7 @@
         <v>8</v>
       </c>
       <c r="D3">
-        <v>200</v>
+        <v>10000</v>
       </c>
       <c r="E3">
         <v>22</v>
@@ -1187,7 +1187,7 @@
         <v>10</v>
       </c>
       <c r="D4">
-        <v>300</v>
+        <v>10000</v>
       </c>
       <c r="E4">
         <v>23</v>
@@ -1204,7 +1204,7 @@
         <v>12</v>
       </c>
       <c r="D5">
-        <v>400</v>
+        <v>10000</v>
       </c>
       <c r="E5">
         <v>24</v>
@@ -1221,7 +1221,7 @@
         <v>14</v>
       </c>
       <c r="D6">
-        <v>500</v>
+        <v>10000</v>
       </c>
       <c r="E6">
         <v>25</v>
@@ -1238,7 +1238,7 @@
         <v>16</v>
       </c>
       <c r="D7">
-        <v>600</v>
+        <v>10000</v>
       </c>
       <c r="E7">
         <v>26</v>
@@ -1255,7 +1255,7 @@
         <v>18</v>
       </c>
       <c r="D8">
-        <v>700</v>
+        <v>10000</v>
       </c>
       <c r="E8">
         <v>27</v>
@@ -1272,7 +1272,7 @@
         <v>20</v>
       </c>
       <c r="D9">
-        <v>800</v>
+        <v>10000</v>
       </c>
       <c r="E9">
         <v>28</v>
@@ -1289,7 +1289,7 @@
         <v>22</v>
       </c>
       <c r="D10">
-        <v>900</v>
+        <v>10000</v>
       </c>
       <c r="E10">
         <v>29</v>
@@ -1306,7 +1306,7 @@
         <v>24</v>
       </c>
       <c r="D11">
-        <v>100</v>
+        <v>10000</v>
       </c>
       <c r="E11">
         <v>30</v>
@@ -1381,7 +1381,7 @@
   <sheetPr/>
   <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
disable doctor, thief and policeman jobs
</commit_message>
<xml_diff>
--- a/app/scripts/data/jobs.xlsx
+++ b/app/scripts/data/jobs.xlsx
@@ -4,19 +4,32 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="20700" windowHeight="9870"/>
+    <workbookView windowWidth="21705" windowHeight="8535"/>
   </bookViews>
   <sheets>
     <sheet name="jobs" sheetId="1" r:id="rId1"/>
     <sheet name="skills" sheetId="3" r:id="rId2"/>
     <sheet name="notices" sheetId="4" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="43">
   <si>
     <t>No</t>
   </si>
@@ -31,6 +44,15 @@
   </si>
   <si>
     <t>Speed</t>
+  </si>
+  <si>
+    <t>Enabled</t>
+  </si>
+  <si>
+    <t>beginner</t>
+  </si>
+  <si>
+    <t>no job</t>
   </si>
   <si>
     <t>miner</t>
@@ -141,7 +163,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="xr9">
   <numFmts count="4">
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
@@ -1112,20 +1134,20 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:D11"/>
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelCol="4"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelCol="5"/>
   <cols>
     <col min="2" max="2" width="10.1428571428571" customWidth="1"/>
     <col min="3" max="3" width="47.4285714285714" customWidth="1"/>
     <col min="4" max="4" width="10.7142857142857" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" s="1" customFormat="1" spans="1:5">
+    <row r="1" s="1" customFormat="1" spans="1:6">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1141,175 +1163,228 @@
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:5">
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
       <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <v>10</v>
+      </c>
+      <c r="F2" t="b">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2">
-        <v>10000</v>
-      </c>
-      <c r="E2">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5">
+    </row>
+    <row r="3" spans="1:6">
       <c r="A3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C3" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D3">
         <v>10000</v>
       </c>
       <c r="E3">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5">
+        <v>21</v>
+      </c>
+      <c r="F3" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
       <c r="A4">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D4">
         <v>10000</v>
       </c>
       <c r="E4">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5">
+        <v>22</v>
+      </c>
+      <c r="F4" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
       <c r="A5">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C5" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D5">
         <v>10000</v>
       </c>
       <c r="E5">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5">
+        <v>23</v>
+      </c>
+      <c r="F5" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
       <c r="A6">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C6" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D6">
         <v>10000</v>
       </c>
       <c r="E6">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5">
+        <v>24</v>
+      </c>
+      <c r="F6" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
       <c r="A7">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C7" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D7">
         <v>10000</v>
       </c>
       <c r="E7">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5">
+        <v>25</v>
+      </c>
+      <c r="F7" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
       <c r="A8">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C8" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D8">
         <v>10000</v>
       </c>
       <c r="E8">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5">
+        <v>26</v>
+      </c>
+      <c r="F8" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
       <c r="A9">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C9" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D9">
         <v>10000</v>
       </c>
       <c r="E9">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5">
+        <v>27</v>
+      </c>
+      <c r="F9" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
       <c r="A10">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C10" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D10">
         <v>10000</v>
       </c>
       <c r="E10">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5">
+        <v>28</v>
+      </c>
+      <c r="F10" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
       <c r="A11">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C11" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D11">
         <v>10000</v>
       </c>
       <c r="E11">
+        <v>29</v>
+      </c>
+      <c r="F11" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12">
+        <v>10</v>
+      </c>
+      <c r="B12" t="s">
+        <v>26</v>
+      </c>
+      <c r="C12" t="s">
+        <v>27</v>
+      </c>
+      <c r="D12">
+        <v>10000</v>
+      </c>
+      <c r="E12">
         <v>30</v>
+      </c>
+      <c r="F12" t="b">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -1341,16 +1416,16 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -1358,16 +1433,16 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="C2" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="D2" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="E2" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
     </row>
   </sheetData>
@@ -1395,13 +1470,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -1409,13 +1484,13 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="C2" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="D2" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -1423,13 +1498,13 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="C3" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="D3" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update job id to job name in get info api
</commit_message>
<xml_diff>
--- a/app/scripts/data/jobs.xlsx
+++ b/app/scripts/data/jobs.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="41">
   <si>
     <t>No</t>
   </si>
@@ -47,12 +47,6 @@
   </si>
   <si>
     <t>Enabled</t>
-  </si>
-  <si>
-    <t>beginner</t>
-  </si>
-  <si>
-    <t>no job</t>
   </si>
   <si>
     <t>miner</t>
@@ -1134,10 +1128,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:F12"/>
+  <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelCol="5"/>
@@ -1169,7 +1163,7 @@
     </row>
     <row r="2" spans="1:6">
       <c r="A2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B2" t="s">
         <v>6</v>
@@ -1178,10 +1172,10 @@
         <v>7</v>
       </c>
       <c r="D2">
-        <v>0</v>
+        <v>10000</v>
       </c>
       <c r="E2">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="F2" t="b">
         <v>1</v>
@@ -1189,7 +1183,7 @@
     </row>
     <row r="3" spans="1:6">
       <c r="A3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B3" t="s">
         <v>8</v>
@@ -1201,7 +1195,7 @@
         <v>10000</v>
       </c>
       <c r="E3">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="F3" t="b">
         <v>1</v>
@@ -1209,7 +1203,7 @@
     </row>
     <row r="4" spans="1:6">
       <c r="A4">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B4" t="s">
         <v>10</v>
@@ -1221,7 +1215,7 @@
         <v>10000</v>
       </c>
       <c r="E4">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="F4" t="b">
         <v>1</v>
@@ -1229,7 +1223,7 @@
     </row>
     <row r="5" spans="1:6">
       <c r="A5">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B5" t="s">
         <v>12</v>
@@ -1241,15 +1235,15 @@
         <v>10000</v>
       </c>
       <c r="E5">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="F5" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:6">
       <c r="A6">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B6" t="s">
         <v>14</v>
@@ -1261,7 +1255,7 @@
         <v>10000</v>
       </c>
       <c r="E6">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="F6" t="b">
         <v>0</v>
@@ -1269,7 +1263,7 @@
     </row>
     <row r="7" spans="1:6">
       <c r="A7">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B7" t="s">
         <v>16</v>
@@ -1281,7 +1275,7 @@
         <v>10000</v>
       </c>
       <c r="E7">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="F7" t="b">
         <v>0</v>
@@ -1289,7 +1283,7 @@
     </row>
     <row r="8" spans="1:6">
       <c r="A8">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B8" t="s">
         <v>18</v>
@@ -1301,15 +1295,15 @@
         <v>10000</v>
       </c>
       <c r="E8">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="F8" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:6">
       <c r="A9">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B9" t="s">
         <v>20</v>
@@ -1321,7 +1315,7 @@
         <v>10000</v>
       </c>
       <c r="E9">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="F9" t="b">
         <v>1</v>
@@ -1329,7 +1323,7 @@
     </row>
     <row r="10" spans="1:6">
       <c r="A10">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B10" t="s">
         <v>22</v>
@@ -1341,7 +1335,7 @@
         <v>10000</v>
       </c>
       <c r="E10">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="F10" t="b">
         <v>1</v>
@@ -1349,7 +1343,7 @@
     </row>
     <row r="11" spans="1:6">
       <c r="A11">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B11" t="s">
         <v>24</v>
@@ -1361,29 +1355,9 @@
         <v>10000</v>
       </c>
       <c r="E11">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F11" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6">
-      <c r="A12">
-        <v>10</v>
-      </c>
-      <c r="B12" t="s">
-        <v>26</v>
-      </c>
-      <c r="C12" t="s">
-        <v>27</v>
-      </c>
-      <c r="D12">
-        <v>10000</v>
-      </c>
-      <c r="E12">
-        <v>30</v>
-      </c>
-      <c r="F12" t="b">
         <v>1</v>
       </c>
     </row>
@@ -1416,16 +1390,16 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -1433,16 +1407,16 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" t="s">
         <v>31</v>
-      </c>
-      <c r="C2" t="s">
-        <v>32</v>
-      </c>
-      <c r="D2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E2" t="s">
-        <v>33</v>
       </c>
     </row>
   </sheetData>
@@ -1470,13 +1444,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>34</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -1484,13 +1458,13 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C2" t="s">
+        <v>36</v>
+      </c>
+      <c r="D2" t="s">
         <v>37</v>
-      </c>
-      <c r="C2" t="s">
-        <v>38</v>
-      </c>
-      <c r="D2" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -1498,13 +1472,13 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C3" t="s">
+        <v>39</v>
+      </c>
+      <c r="D3" t="s">
         <v>40</v>
-      </c>
-      <c r="C3" t="s">
-        <v>41</v>
-      </c>
-      <c r="D3" t="s">
-        <v>42</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update notification api and script
</commit_message>
<xml_diff>
--- a/app/scripts/data/jobs.xlsx
+++ b/app/scripts/data/jobs.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="21705" windowHeight="8535"/>
+    <workbookView windowWidth="20895" windowHeight="10560" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="jobs" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="45">
   <si>
     <t>No</t>
   </si>
@@ -127,6 +127,9 @@
     <t>breaks wall</t>
   </si>
   <si>
+    <t>Name</t>
+  </si>
+  <si>
     <t>Contents</t>
   </si>
   <si>
@@ -136,6 +139,9 @@
     <t>Is Available</t>
   </si>
   <si>
+    <t>Alarm</t>
+  </si>
+  <si>
     <t>Coming up New Job Item</t>
   </si>
   <si>
@@ -152,6 +158,12 @@
   </si>
   <si>
     <t>no</t>
+  </si>
+  <si>
+    <t>Summer event</t>
+  </si>
+  <si>
+    <t>Upcoming 2024 Summer map</t>
   </si>
 </sst>
 </file>
@@ -1130,8 +1142,8 @@
   <sheetPr/>
   <dimension ref="A1:F11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelCol="5"/>
@@ -1428,18 +1440,19 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="2" outlineLevelCol="3"/>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="3" outlineLevelCol="4"/>
   <cols>
-    <col min="2" max="2" width="22.4285714285714" customWidth="1"/>
+    <col min="2" max="2" width="15.4285714285714" customWidth="1"/>
+    <col min="3" max="3" width="35.5714285714286" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" s="1" customFormat="1" spans="1:4">
+    <row r="1" s="1" customFormat="1" spans="1:5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1452,33 +1465,59 @@
       <c r="D1" s="1" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="2" spans="1:4">
+      <c r="E1" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C2" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D2" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4">
+        <v>38</v>
+      </c>
+      <c r="E2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C3" t="s">
+        <v>40</v>
+      </c>
+      <c r="D3" t="s">
+        <v>41</v>
+      </c>
+      <c r="E3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>43</v>
+      </c>
+      <c r="C4" t="s">
+        <v>44</v>
+      </c>
+      <c r="D4" t="s">
+        <v>41</v>
+      </c>
+      <c r="E4" t="s">
         <v>39</v>
-      </c>
-      <c r="D3" t="s">
-        <v>40</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add start_date and end_date in notice
</commit_message>
<xml_diff>
--- a/app/scripts/data/jobs.xlsx
+++ b/app/scripts/data/jobs.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="47">
   <si>
     <t>No</t>
   </si>
@@ -134,6 +134,12 @@
   </si>
   <si>
     <t>Type</t>
+  </si>
+  <si>
+    <t>Start Date</t>
+  </si>
+  <si>
+    <t>End Date</t>
   </si>
   <si>
     <t>Is Available</t>
@@ -170,11 +176,12 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="xr9">
-  <numFmts count="4">
+  <numFmts count="5">
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="m/d/yyyy;@"/>
   </numFmts>
   <fonts count="21">
     <font>
@@ -791,9 +798,15 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="178" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1440,19 +1453,21 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="3" outlineLevelCol="4"/>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="3" outlineLevelCol="6"/>
   <cols>
     <col min="2" max="2" width="15.4285714285714" customWidth="1"/>
     <col min="3" max="3" width="35.5714285714286" customWidth="1"/>
+    <col min="5" max="5" width="14.8571428571429" style="2" customWidth="1"/>
+    <col min="6" max="6" width="17.7142857142857" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" s="1" customFormat="1" spans="1:5">
+    <row r="1" s="1" customFormat="1" spans="1:7">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1465,59 +1480,81 @@
       <c r="D1" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="3" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="2" spans="1:5">
+      <c r="F1" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="C2" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="D2" t="s">
-        <v>38</v>
-      </c>
-      <c r="E2" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5">
+        <v>40</v>
+      </c>
+      <c r="E2" s="2">
+        <v>45627</v>
+      </c>
+      <c r="F2" s="2"/>
+      <c r="G2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="C3" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="D3" t="s">
-        <v>41</v>
-      </c>
-      <c r="E3" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5">
+        <v>43</v>
+      </c>
+      <c r="E3" s="2">
+        <v>45628</v>
+      </c>
+      <c r="F3" s="2">
+        <v>45657</v>
+      </c>
+      <c r="G3" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
+        <v>45</v>
+      </c>
+      <c r="C4" t="s">
+        <v>46</v>
+      </c>
+      <c r="D4" t="s">
         <v>43</v>
       </c>
-      <c r="C4" t="s">
-        <v>44</v>
-      </c>
-      <c r="D4" t="s">
+      <c r="E4" s="2">
+        <v>45474</v>
+      </c>
+      <c r="F4" s="2">
+        <v>45565</v>
+      </c>
+      <c r="G4" t="s">
         <v>41</v>
-      </c>
-      <c r="E4" t="s">
-        <v>39</v>
       </c>
     </row>
   </sheetData>

</xml_diff>